<commit_message>
fix bug upload sudoku
</commit_message>
<xml_diff>
--- a/test/puzzle.xlsx
+++ b/test/puzzle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndresDelgadillo\PycharmProjects\dash_client\sudoku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndresDelgadillo\PycharmProjects\dash_client\sudoku\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B8AA070-1BC8-4B71-A2F2-2B9F3D30AF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C5C96C-D2FB-437E-A715-F33AAC409123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1FB607B2-A504-487B-B3C1-DE8A7BE48132}"/>
   </bookViews>
@@ -35,10 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -58,7 +54,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -66,12 +62,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,265 +498,169 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>2</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
         <v>6</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>5</v>
       </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="1">
         <v>4</v>
       </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
+      <c r="H1" s="2"/>
+      <c r="I1" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6">
         <v>9</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5">
         <v>3</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="8"/>
+      <c r="F3" s="9">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3">
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="5"/>
+      <c r="F5" s="6">
         <v>6</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>7</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="5"/>
+      <c r="I5" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="8"/>
+      <c r="I6" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>9</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="2"/>
+      <c r="I7" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="5"/>
+      <c r="F8" s="6">
         <v>3</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5">
         <v>6</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>